<commit_message>
Object_Spawn_Table과 Object_Table에 Next Point, End Point 구분
7. Next Point - 동일 스테이지에서 다음 맵으로 넘어가는 워프
8. End Point - 스테이지가 종료되는 워프
</commit_message>
<xml_diff>
--- a/GameDesign/Table/TurtleBomb_Object_Spawn_Table.xlsx
+++ b/GameDesign/Table/TurtleBomb_Object_Spawn_Table.xlsx
@@ -615,7 +615,7 @@
     <cellStyle name="표준" xfId="0" builtinId="0"/>
     <cellStyle name="표준 3" xfId="1"/>
   </cellStyles>
-  <dxfs count="147">
+  <dxfs count="15">
     <dxf>
       <fill>
         <patternFill>
@@ -666,6 +666,23 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
@@ -704,944 +721,6 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1935,7 +1014,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="V145" sqref="V145"/>
+      <selection pane="bottomRight" activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2193,7 +1272,7 @@
         <v>0</v>
       </c>
       <c r="T4" s="10">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.45">
@@ -3123,7 +2202,7 @@
         <v>0</v>
       </c>
       <c r="T19" s="10">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.45">
@@ -5396,7 +4475,7 @@
         <v>0</v>
       </c>
       <c r="M56" s="12">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N56" s="12">
         <v>0</v>
@@ -7256,7 +6335,7 @@
         <v>0</v>
       </c>
       <c r="M86" s="12">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N86" s="12">
         <v>0</v>
@@ -9116,7 +8195,7 @@
         <v>1</v>
       </c>
       <c r="M116" s="12">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N116" s="12">
         <v>1</v>
@@ -10976,7 +10055,7 @@
         <v>1</v>
       </c>
       <c r="M146" s="12">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N146" s="12">
         <v>1</v>
@@ -13766,7 +12845,7 @@
         <v>0</v>
       </c>
       <c r="M191" s="12">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N191" s="12">
         <v>0</v>
@@ -16143,7 +15222,7 @@
         <v>0</v>
       </c>
       <c r="T229" s="10">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="230" spans="1:20" x14ac:dyDescent="0.45">
@@ -17947,26 +17026,29 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="F1:T1048576">
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+      <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
TurtleBomb_Adventure_Boss_Table 생성 및 그외 Table/기획서 내용수정
</commit_message>
<xml_diff>
--- a/GameDesign/Table/TurtleBomb_Object_Spawn_Table.xlsx
+++ b/GameDesign/Table/TurtleBomb_Object_Spawn_Table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12290" tabRatio="653"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" tabRatio="653"/>
   </bookViews>
   <sheets>
     <sheet name="Table_Object_Spawn" sheetId="4" r:id="rId1"/>
@@ -615,56 +615,7 @@
     <cellStyle name="표준" xfId="0" builtinId="0"/>
     <cellStyle name="표준 3" xfId="1"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <color theme="0"/>
@@ -1011,23 +962,23 @@
   <dimension ref="A1:T258"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C228" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N14" sqref="N14"/>
+      <selection pane="bottomRight" activeCell="D253" sqref="D253"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="20" width="3.08203125" style="3" customWidth="1"/>
+    <col min="6" max="20" width="3.125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>2</v>
       </c>
@@ -1089,7 +1040,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -1151,7 +1102,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="20" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:20" s="20" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
@@ -1213,7 +1164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="35">
         <v>1</v>
       </c>
@@ -1275,7 +1226,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="39">
         <v>2</v>
       </c>
@@ -1337,7 +1288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="39">
         <v>3</v>
       </c>
@@ -1399,7 +1350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="39">
         <v>4</v>
       </c>
@@ -1461,7 +1412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="39">
         <v>5</v>
       </c>
@@ -1523,7 +1474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="39">
         <v>6</v>
       </c>
@@ -1585,7 +1536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="39">
         <v>7</v>
       </c>
@@ -1647,7 +1598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="39">
         <v>8</v>
       </c>
@@ -1709,7 +1660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="39">
         <v>9</v>
       </c>
@@ -1771,7 +1722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="39">
         <v>10</v>
       </c>
@@ -1833,7 +1784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="39">
         <v>11</v>
       </c>
@@ -1895,7 +1846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="39">
         <v>12</v>
       </c>
@@ -1957,7 +1908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="39">
         <v>13</v>
       </c>
@@ -2019,7 +1970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="39">
         <v>14</v>
       </c>
@@ -2081,7 +2032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" s="7" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:20" s="7" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="40">
         <v>15</v>
       </c>
@@ -2143,7 +2094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="35">
         <v>16</v>
       </c>
@@ -2205,7 +2156,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="39">
         <v>17</v>
       </c>
@@ -2267,7 +2218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="39">
         <v>18</v>
       </c>
@@ -2329,7 +2280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="39">
         <v>19</v>
       </c>
@@ -2391,7 +2342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="39">
         <v>20</v>
       </c>
@@ -2453,7 +2404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="39">
         <v>21</v>
       </c>
@@ -2515,7 +2466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="39">
         <v>22</v>
       </c>
@@ -2577,7 +2528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="39">
         <v>23</v>
       </c>
@@ -2639,7 +2590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="39">
         <v>24</v>
       </c>
@@ -2701,7 +2652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="39">
         <v>25</v>
       </c>
@@ -2763,7 +2714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="39">
         <v>26</v>
       </c>
@@ -2825,7 +2776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="39">
         <v>27</v>
       </c>
@@ -2887,7 +2838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="39">
         <v>28</v>
       </c>
@@ -2949,7 +2900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="39">
         <v>29</v>
       </c>
@@ -3011,7 +2962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="40">
         <v>30</v>
       </c>
@@ -3073,7 +3024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="35">
         <v>31</v>
       </c>
@@ -3135,7 +3086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="39">
         <v>32</v>
       </c>
@@ -3197,7 +3148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" s="39">
         <v>33</v>
       </c>
@@ -3259,7 +3210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" s="39">
         <v>34</v>
       </c>
@@ -3321,7 +3272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" s="39">
         <v>35</v>
       </c>
@@ -3383,7 +3334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="39">
         <v>36</v>
       </c>
@@ -3445,7 +3396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="39">
         <v>37</v>
       </c>
@@ -3507,7 +3458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="39">
         <v>38</v>
       </c>
@@ -3569,7 +3520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="39">
         <v>39</v>
       </c>
@@ -3631,7 +3582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" s="39">
         <v>40</v>
       </c>
@@ -3693,7 +3644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" s="39">
         <v>41</v>
       </c>
@@ -3755,7 +3706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="39">
         <v>42</v>
       </c>
@@ -3817,7 +3768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="39">
         <v>43</v>
       </c>
@@ -3879,7 +3830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" s="39">
         <v>44</v>
       </c>
@@ -3941,7 +3892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="40">
         <v>45</v>
       </c>
@@ -4003,7 +3954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="35">
         <v>46</v>
       </c>
@@ -4065,7 +4016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="39">
         <v>47</v>
       </c>
@@ -4127,7 +4078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="39">
         <v>48</v>
       </c>
@@ -4189,7 +4140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" s="39">
         <v>49</v>
       </c>
@@ -4251,7 +4202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" s="39">
         <v>50</v>
       </c>
@@ -4313,7 +4264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" s="39">
         <v>51</v>
       </c>
@@ -4375,7 +4326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" s="39">
         <v>52</v>
       </c>
@@ -4437,7 +4388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" s="39">
         <v>53</v>
       </c>
@@ -4499,7 +4450,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" s="39">
         <v>54</v>
       </c>
@@ -4561,7 +4512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" s="39">
         <v>55</v>
       </c>
@@ -4623,7 +4574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" s="39">
         <v>56</v>
       </c>
@@ -4685,7 +4636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" s="39">
         <v>57</v>
       </c>
@@ -4747,7 +4698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" s="39">
         <v>58</v>
       </c>
@@ -4809,7 +4760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" s="39">
         <v>59</v>
       </c>
@@ -4871,7 +4822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="40">
         <v>60</v>
       </c>
@@ -4933,7 +4884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" s="35">
         <v>61</v>
       </c>
@@ -4995,7 +4946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A65" s="39">
         <v>62</v>
       </c>
@@ -5057,7 +5008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A66" s="39">
         <v>63</v>
       </c>
@@ -5119,7 +5070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A67" s="39">
         <v>64</v>
       </c>
@@ -5181,7 +5132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A68" s="39">
         <v>65</v>
       </c>
@@ -5243,7 +5194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A69" s="39">
         <v>66</v>
       </c>
@@ -5305,7 +5256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A70" s="39">
         <v>67</v>
       </c>
@@ -5367,7 +5318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A71" s="39">
         <v>68</v>
       </c>
@@ -5429,7 +5380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A72" s="39">
         <v>69</v>
       </c>
@@ -5491,7 +5442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A73" s="39">
         <v>70</v>
       </c>
@@ -5553,7 +5504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A74" s="39">
         <v>71</v>
       </c>
@@ -5615,7 +5566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A75" s="39">
         <v>72</v>
       </c>
@@ -5677,7 +5628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A76" s="39">
         <v>73</v>
       </c>
@@ -5739,7 +5690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A77" s="39">
         <v>74</v>
       </c>
@@ -5801,7 +5752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="40">
         <v>75</v>
       </c>
@@ -5863,7 +5814,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A79" s="35">
         <v>76</v>
       </c>
@@ -5925,7 +5876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A80" s="39">
         <v>77</v>
       </c>
@@ -5987,7 +5938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A81" s="39">
         <v>78</v>
       </c>
@@ -6049,7 +6000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A82" s="39">
         <v>79</v>
       </c>
@@ -6111,7 +6062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A83" s="39">
         <v>80</v>
       </c>
@@ -6173,7 +6124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A84" s="39">
         <v>81</v>
       </c>
@@ -6235,7 +6186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A85" s="39">
         <v>82</v>
       </c>
@@ -6297,7 +6248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A86" s="39">
         <v>83</v>
       </c>
@@ -6359,7 +6310,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A87" s="39">
         <v>84</v>
       </c>
@@ -6421,7 +6372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A88" s="39">
         <v>85</v>
       </c>
@@ -6483,7 +6434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A89" s="39">
         <v>86</v>
       </c>
@@ -6545,7 +6496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A90" s="39">
         <v>87</v>
       </c>
@@ -6607,7 +6558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A91" s="39">
         <v>88</v>
       </c>
@@ -6669,7 +6620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A92" s="39">
         <v>89</v>
       </c>
@@ -6731,7 +6682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="40">
         <v>90</v>
       </c>
@@ -6793,7 +6744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A94" s="35">
         <v>91</v>
       </c>
@@ -6855,7 +6806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A95" s="39">
         <v>92</v>
       </c>
@@ -6917,7 +6868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A96" s="39">
         <v>93</v>
       </c>
@@ -6979,7 +6930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A97" s="39">
         <v>94</v>
       </c>
@@ -7041,7 +6992,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A98" s="39">
         <v>95</v>
       </c>
@@ -7103,7 +7054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A99" s="39">
         <v>96</v>
       </c>
@@ -7165,7 +7116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A100" s="39">
         <v>97</v>
       </c>
@@ -7227,7 +7178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A101" s="39">
         <v>98</v>
       </c>
@@ -7289,7 +7240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A102" s="39">
         <v>99</v>
       </c>
@@ -7351,7 +7302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A103" s="39">
         <v>100</v>
       </c>
@@ -7413,7 +7364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A104" s="39">
         <v>101</v>
       </c>
@@ -7475,7 +7426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A105" s="39">
         <v>102</v>
       </c>
@@ -7537,7 +7488,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A106" s="39">
         <v>103</v>
       </c>
@@ -7599,7 +7550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A107" s="39">
         <v>104</v>
       </c>
@@ -7661,7 +7612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="40">
         <v>105</v>
       </c>
@@ -7723,7 +7674,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A109" s="35">
         <v>106</v>
       </c>
@@ -7785,7 +7736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A110" s="39">
         <v>107</v>
       </c>
@@ -7847,7 +7798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A111" s="39">
         <v>108</v>
       </c>
@@ -7909,7 +7860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A112" s="39">
         <v>109</v>
       </c>
@@ -7971,7 +7922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A113" s="39">
         <v>110</v>
       </c>
@@ -8033,7 +7984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A114" s="39">
         <v>111</v>
       </c>
@@ -8095,7 +8046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A115" s="39">
         <v>112</v>
       </c>
@@ -8157,7 +8108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A116" s="39">
         <v>113</v>
       </c>
@@ -8219,7 +8170,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A117" s="39">
         <v>114</v>
       </c>
@@ -8281,7 +8232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A118" s="39">
         <v>115</v>
       </c>
@@ -8343,7 +8294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A119" s="39">
         <v>116</v>
       </c>
@@ -8405,7 +8356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A120" s="39">
         <v>117</v>
       </c>
@@ -8467,7 +8418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A121" s="39">
         <v>118</v>
       </c>
@@ -8529,7 +8480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A122" s="39">
         <v>119</v>
       </c>
@@ -8591,7 +8542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="40">
         <v>120</v>
       </c>
@@ -8653,7 +8604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A124" s="35">
         <v>121</v>
       </c>
@@ -8715,7 +8666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A125" s="39">
         <v>122</v>
       </c>
@@ -8777,7 +8728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A126" s="39">
         <v>123</v>
       </c>
@@ -8839,7 +8790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A127" s="39">
         <v>124</v>
       </c>
@@ -8901,7 +8852,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A128" s="39">
         <v>125</v>
       </c>
@@ -8963,7 +8914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A129" s="39">
         <v>126</v>
       </c>
@@ -9025,7 +8976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A130" s="39">
         <v>127</v>
       </c>
@@ -9087,7 +9038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A131" s="39">
         <v>128</v>
       </c>
@@ -9149,7 +9100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A132" s="39">
         <v>129</v>
       </c>
@@ -9211,7 +9162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A133" s="39">
         <v>130</v>
       </c>
@@ -9273,7 +9224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A134" s="39">
         <v>131</v>
       </c>
@@ -9335,7 +9286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A135" s="39">
         <v>132</v>
       </c>
@@ -9397,7 +9348,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A136" s="39">
         <v>133</v>
       </c>
@@ -9459,7 +9410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A137" s="39">
         <v>134</v>
       </c>
@@ -9521,7 +9472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:20" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="138" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A138" s="40">
         <v>135</v>
       </c>
@@ -9583,7 +9534,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="139" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A139" s="35">
         <v>136</v>
       </c>
@@ -9645,7 +9596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A140" s="39">
         <v>137</v>
       </c>
@@ -9707,7 +9658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A141" s="39">
         <v>138</v>
       </c>
@@ -9769,7 +9720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A142" s="39">
         <v>139</v>
       </c>
@@ -9831,7 +9782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A143" s="39">
         <v>140</v>
       </c>
@@ -9893,7 +9844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A144" s="39">
         <v>141</v>
       </c>
@@ -9955,7 +9906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A145" s="39">
         <v>142</v>
       </c>
@@ -10017,7 +9968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A146" s="39">
         <v>143</v>
       </c>
@@ -10079,7 +10030,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="147" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A147" s="39">
         <v>144</v>
       </c>
@@ -10141,7 +10092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A148" s="39">
         <v>145</v>
       </c>
@@ -10203,7 +10154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A149" s="39">
         <v>146</v>
       </c>
@@ -10265,7 +10216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A150" s="39">
         <v>147</v>
       </c>
@@ -10327,7 +10278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A151" s="39">
         <v>148</v>
       </c>
@@ -10389,7 +10340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A152" s="39">
         <v>149</v>
       </c>
@@ -10451,7 +10402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:20" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="153" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A153" s="40">
         <v>150</v>
       </c>
@@ -10513,7 +10464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A154" s="35">
         <v>151</v>
       </c>
@@ -10575,7 +10526,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="155" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A155" s="39">
         <v>152</v>
       </c>
@@ -10637,7 +10588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A156" s="39">
         <v>153</v>
       </c>
@@ -10699,7 +10650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A157" s="39">
         <v>154</v>
       </c>
@@ -10761,7 +10712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A158" s="39">
         <v>155</v>
       </c>
@@ -10823,7 +10774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A159" s="39">
         <v>156</v>
       </c>
@@ -10885,7 +10836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A160" s="39">
         <v>157</v>
       </c>
@@ -10947,7 +10898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A161" s="39">
         <v>158</v>
       </c>
@@ -11009,7 +10960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A162" s="39">
         <v>159</v>
       </c>
@@ -11071,7 +11022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A163" s="39">
         <v>160</v>
       </c>
@@ -11133,7 +11084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A164" s="39">
         <v>161</v>
       </c>
@@ -11195,7 +11146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A165" s="39">
         <v>162</v>
       </c>
@@ -11257,7 +11208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A166" s="39">
         <v>163</v>
       </c>
@@ -11319,7 +11270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A167" s="39">
         <v>164</v>
       </c>
@@ -11381,7 +11332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="168" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A168" s="40">
         <v>165</v>
       </c>
@@ -11443,7 +11394,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="169" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A169" s="35">
         <v>166</v>
       </c>
@@ -11505,7 +11456,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="170" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A170" s="39">
         <v>167</v>
       </c>
@@ -11567,7 +11518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A171" s="39">
         <v>168</v>
       </c>
@@ -11629,7 +11580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A172" s="39">
         <v>169</v>
       </c>
@@ -11691,7 +11642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A173" s="39">
         <v>170</v>
       </c>
@@ -11753,7 +11704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A174" s="39">
         <v>171</v>
       </c>
@@ -11815,7 +11766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A175" s="39">
         <v>172</v>
       </c>
@@ -11877,7 +11828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A176" s="39">
         <v>173</v>
       </c>
@@ -11939,7 +11890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="177" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A177" s="39">
         <v>174</v>
       </c>
@@ -12001,7 +11952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A178" s="39">
         <v>175</v>
       </c>
@@ -12063,7 +12014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A179" s="39">
         <v>176</v>
       </c>
@@ -12125,7 +12076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A180" s="39">
         <v>177</v>
       </c>
@@ -12187,7 +12138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A181" s="39">
         <v>178</v>
       </c>
@@ -12249,7 +12200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A182" s="39">
         <v>179</v>
       </c>
@@ -12311,7 +12262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:20" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="183" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A183" s="40">
         <v>180</v>
       </c>
@@ -12373,7 +12324,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="184" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A184" s="35">
         <v>181</v>
       </c>
@@ -12435,7 +12386,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="185" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A185" s="39">
         <v>182</v>
       </c>
@@ -12497,7 +12448,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="186" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A186" s="39">
         <v>183</v>
       </c>
@@ -12559,7 +12510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A187" s="39">
         <v>184</v>
       </c>
@@ -12621,7 +12572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A188" s="39">
         <v>185</v>
       </c>
@@ -12683,7 +12634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A189" s="39">
         <v>186</v>
       </c>
@@ -12745,7 +12696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A190" s="39">
         <v>187</v>
       </c>
@@ -12807,7 +12758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A191" s="39">
         <v>188</v>
       </c>
@@ -12869,7 +12820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A192" s="39">
         <v>189</v>
       </c>
@@ -12931,7 +12882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A193" s="39">
         <v>190</v>
       </c>
@@ -12993,7 +12944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A194" s="39">
         <v>191</v>
       </c>
@@ -13055,7 +13006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A195" s="39">
         <v>192</v>
       </c>
@@ -13117,7 +13068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A196" s="39">
         <v>193</v>
       </c>
@@ -13179,7 +13130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A197" s="39">
         <v>194</v>
       </c>
@@ -13241,7 +13192,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="198" spans="1:20" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="198" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A198" s="40">
         <v>195</v>
       </c>
@@ -13303,7 +13254,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="199" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A199" s="35">
         <v>196</v>
       </c>
@@ -13365,7 +13316,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="200" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A200" s="39">
         <v>197</v>
       </c>
@@ -13427,7 +13378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A201" s="39">
         <v>198</v>
       </c>
@@ -13489,7 +13440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A202" s="39">
         <v>199</v>
       </c>
@@ -13551,7 +13502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A203" s="39">
         <v>200</v>
       </c>
@@ -13613,7 +13564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A204" s="39">
         <v>201</v>
       </c>
@@ -13675,7 +13626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A205" s="39">
         <v>202</v>
       </c>
@@ -13737,7 +13688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A206" s="39">
         <v>203</v>
       </c>
@@ -13799,7 +13750,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="207" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A207" s="39">
         <v>204</v>
       </c>
@@ -13861,7 +13812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A208" s="39">
         <v>205</v>
       </c>
@@ -13923,7 +13874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A209" s="39">
         <v>206</v>
       </c>
@@ -13985,7 +13936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A210" s="39">
         <v>207</v>
       </c>
@@ -14047,7 +13998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A211" s="39">
         <v>208</v>
       </c>
@@ -14109,7 +14060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A212" s="39">
         <v>209</v>
       </c>
@@ -14171,7 +14122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:20" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="213" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A213" s="40">
         <v>210</v>
       </c>
@@ -14233,7 +14184,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="214" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A214" s="35">
         <v>211</v>
       </c>
@@ -14295,7 +14246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A215" s="39">
         <v>212</v>
       </c>
@@ -14357,7 +14308,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="216" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A216" s="39">
         <v>213</v>
       </c>
@@ -14419,7 +14370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A217" s="39">
         <v>214</v>
       </c>
@@ -14481,7 +14432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A218" s="39">
         <v>215</v>
       </c>
@@ -14543,7 +14494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A219" s="39">
         <v>216</v>
       </c>
@@ -14605,7 +14556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A220" s="39">
         <v>217</v>
       </c>
@@ -14667,7 +14618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A221" s="39">
         <v>218</v>
       </c>
@@ -14729,7 +14680,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="222" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A222" s="39">
         <v>219</v>
       </c>
@@ -14791,7 +14742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A223" s="39">
         <v>220</v>
       </c>
@@ -14853,7 +14804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A224" s="39">
         <v>221</v>
       </c>
@@ -14915,7 +14866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A225" s="39">
         <v>222</v>
       </c>
@@ -14977,7 +14928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A226" s="39">
         <v>223</v>
       </c>
@@ -15039,7 +14990,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="227" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A227" s="39">
         <v>224</v>
       </c>
@@ -15101,7 +15052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:20" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="228" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A228" s="40">
         <v>225</v>
       </c>
@@ -15163,7 +15114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A229" s="35">
         <v>226</v>
       </c>
@@ -15225,7 +15176,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="230" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A230" s="39">
         <v>227</v>
       </c>
@@ -15287,7 +15238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A231" s="39">
         <v>228</v>
       </c>
@@ -15349,7 +15300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A232" s="39">
         <v>229</v>
       </c>
@@ -15411,7 +15362,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="233" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A233" s="39">
         <v>230</v>
       </c>
@@ -15473,7 +15424,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="234" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A234" s="39">
         <v>231</v>
       </c>
@@ -15535,7 +15486,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="235" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A235" s="39">
         <v>232</v>
       </c>
@@ -15597,7 +15548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="236" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A236" s="39">
         <v>233</v>
       </c>
@@ -15659,7 +15610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="237" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A237" s="39">
         <v>234</v>
       </c>
@@ -15721,7 +15672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="238" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A238" s="39">
         <v>235</v>
       </c>
@@ -15783,7 +15734,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="239" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A239" s="39">
         <v>236</v>
       </c>
@@ -15845,7 +15796,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="240" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A240" s="39">
         <v>237</v>
       </c>
@@ -15907,7 +15858,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="241" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A241" s="39">
         <v>238</v>
       </c>
@@ -15969,7 +15920,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="242" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A242" s="39">
         <v>239</v>
       </c>
@@ -16031,7 +15982,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="243" spans="1:20" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="243" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A243" s="40">
         <v>240</v>
       </c>
@@ -16093,7 +16044,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="244" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A244" s="35">
         <v>241</v>
       </c>
@@ -16131,7 +16082,7 @@
         <v>0</v>
       </c>
       <c r="M244" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N244" s="9">
         <v>0</v>
@@ -16155,7 +16106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A245" s="39">
         <v>242</v>
       </c>
@@ -16175,7 +16126,7 @@
         <v>0</v>
       </c>
       <c r="G245" s="12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H245" s="12">
         <v>0</v>
@@ -16193,7 +16144,7 @@
         <v>0</v>
       </c>
       <c r="M245" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N245" s="12">
         <v>0</v>
@@ -16211,13 +16162,13 @@
         <v>0</v>
       </c>
       <c r="S245" s="12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="T245" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A246" s="39">
         <v>243</v>
       </c>
@@ -16243,7 +16194,7 @@
         <v>0</v>
       </c>
       <c r="I246" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J246" s="12">
         <v>0</v>
@@ -16252,13 +16203,13 @@
         <v>0</v>
       </c>
       <c r="L246" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M246" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N246" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O246" s="12">
         <v>0</v>
@@ -16267,7 +16218,7 @@
         <v>0</v>
       </c>
       <c r="Q246" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R246" s="12">
         <v>0</v>
@@ -16279,7 +16230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A247" s="39">
         <v>244</v>
       </c>
@@ -16302,10 +16253,10 @@
         <v>1</v>
       </c>
       <c r="H247" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I247" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J247" s="12">
         <v>0</v>
@@ -16329,10 +16280,10 @@
         <v>0</v>
       </c>
       <c r="Q247" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R247" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S247" s="12">
         <v>1</v>
@@ -16341,7 +16292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A248" s="39">
         <v>245</v>
       </c>
@@ -16379,7 +16330,7 @@
         <v>0</v>
       </c>
       <c r="M248" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N248" s="12">
         <v>0</v>
@@ -16403,7 +16354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A249" s="39">
         <v>246</v>
       </c>
@@ -16423,7 +16374,7 @@
         <v>0</v>
       </c>
       <c r="G249" s="12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H249" s="12">
         <v>0</v>
@@ -16441,7 +16392,7 @@
         <v>0</v>
       </c>
       <c r="M249" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N249" s="12">
         <v>0</v>
@@ -16459,13 +16410,13 @@
         <v>0</v>
       </c>
       <c r="S249" s="12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="T249" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A250" s="39">
         <v>247</v>
       </c>
@@ -16488,7 +16439,7 @@
         <v>0</v>
       </c>
       <c r="H250" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I250" s="12">
         <v>0</v>
@@ -16500,13 +16451,13 @@
         <v>0</v>
       </c>
       <c r="L250" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M250" s="12">
         <v>0</v>
       </c>
       <c r="N250" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O250" s="12">
         <v>0</v>
@@ -16518,7 +16469,7 @@
         <v>0</v>
       </c>
       <c r="R250" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S250" s="12">
         <v>0</v>
@@ -16527,7 +16478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A251" s="39">
         <v>248</v>
       </c>
@@ -16547,19 +16498,19 @@
         <v>0</v>
       </c>
       <c r="G251" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H251" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I251" s="12">
         <v>0</v>
       </c>
       <c r="J251" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K251" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L251" s="12">
         <v>0</v>
@@ -16571,25 +16522,25 @@
         <v>0</v>
       </c>
       <c r="O251" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P251" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q251" s="12">
         <v>0</v>
       </c>
       <c r="R251" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S251" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T251" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A252" s="39">
         <v>249</v>
       </c>
@@ -16612,7 +16563,7 @@
         <v>0</v>
       </c>
       <c r="H252" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I252" s="12">
         <v>0</v>
@@ -16624,13 +16575,13 @@
         <v>0</v>
       </c>
       <c r="L252" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M252" s="12">
         <v>0</v>
       </c>
       <c r="N252" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O252" s="12">
         <v>0</v>
@@ -16642,7 +16593,7 @@
         <v>0</v>
       </c>
       <c r="R252" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S252" s="12">
         <v>0</v>
@@ -16651,7 +16602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A253" s="39">
         <v>250</v>
       </c>
@@ -16671,7 +16622,7 @@
         <v>0</v>
       </c>
       <c r="G253" s="12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H253" s="12">
         <v>0</v>
@@ -16689,7 +16640,7 @@
         <v>0</v>
       </c>
       <c r="M253" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N253" s="12">
         <v>0</v>
@@ -16707,13 +16658,13 @@
         <v>0</v>
       </c>
       <c r="S253" s="12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="T253" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A254" s="39">
         <v>251</v>
       </c>
@@ -16751,7 +16702,7 @@
         <v>0</v>
       </c>
       <c r="M254" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N254" s="12">
         <v>0</v>
@@ -16775,7 +16726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A255" s="39">
         <v>252</v>
       </c>
@@ -16798,10 +16749,10 @@
         <v>1</v>
       </c>
       <c r="H255" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I255" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J255" s="12">
         <v>0</v>
@@ -16825,10 +16776,10 @@
         <v>0</v>
       </c>
       <c r="Q255" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R255" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S255" s="12">
         <v>1</v>
@@ -16837,7 +16788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A256" s="39">
         <v>253</v>
       </c>
@@ -16863,7 +16814,7 @@
         <v>0</v>
       </c>
       <c r="I256" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J256" s="12">
         <v>0</v>
@@ -16872,13 +16823,13 @@
         <v>0</v>
       </c>
       <c r="L256" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M256" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N256" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O256" s="12">
         <v>0</v>
@@ -16887,7 +16838,7 @@
         <v>0</v>
       </c>
       <c r="Q256" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R256" s="12">
         <v>0</v>
@@ -16899,7 +16850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="257" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A257" s="39">
         <v>254</v>
       </c>
@@ -16937,7 +16888,7 @@
         <v>0</v>
       </c>
       <c r="M257" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N257" s="12">
         <v>0</v>
@@ -16955,13 +16906,13 @@
         <v>0</v>
       </c>
       <c r="S257" s="12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="T257" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:20" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="258" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A258" s="40">
         <v>255</v>
       </c>
@@ -16999,7 +16950,7 @@
         <v>0</v>
       </c>
       <c r="M258" s="15">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N258" s="15">
         <v>0</v>
@@ -17026,28 +16977,28 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="F1:T1048576">
-    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>